<commit_message>
Add signal for the out door
</commit_message>
<xml_diff>
--- a/Cabinets/OfficeCabinet_Type1_L1_3P/datasheets/Signals.xlsx
+++ b/Cabinets/OfficeCabinet_Type1_L1_3P/datasheets/Signals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\POLYGONTeam\Documents\QET\RoomCabinet3P\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\POLYGONTeam\Documents\Git\ztm_doc\Cabinets\OfficeCabinet_Type1_L1_3P\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22321680-3A07-48C4-9A11-B48A50AC7F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D779BD-8E3F-4120-9D97-AE67F741F98C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B7F42A5-FF45-4201-A870-3B1FC62E9821}"/>
+    <workbookView xWindow="3105" yWindow="0" windowWidth="25695" windowHeight="15600" xr2:uid="{1B7F42A5-FF45-4201-A870-3B1FC62E9821}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="149">
   <si>
     <t>№</t>
   </si>
@@ -463,6 +463,15 @@
   </si>
   <si>
     <t>8.16</t>
+  </si>
+  <si>
+    <t>ODT</t>
+  </si>
+  <si>
+    <t>Out Door Tamper</t>
+  </si>
+  <si>
+    <t>12.1</t>
   </si>
 </sst>
 </file>
@@ -835,7 +844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A60837-B00C-4F34-AD1F-3B3A0436DA02}">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
       <selection activeCell="A53" sqref="A53:F78"/>
     </sheetView>
   </sheetViews>
@@ -2161,61 +2170,87 @@
       <c r="A67">
         <v>64</v>
       </c>
+      <c r="B67" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>65</v>
       </c>
+      <c r="B68" s="1"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>66</v>
       </c>
+      <c r="B69" s="1"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>67</v>
       </c>
+      <c r="B70" s="1"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>68</v>
       </c>
+      <c r="B71" s="1"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>69</v>
       </c>
+      <c r="B72" s="1"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>70</v>
       </c>
+      <c r="B73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>71</v>
       </c>
+      <c r="B74" s="1"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>72</v>
       </c>
+      <c r="B75" s="1"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>73</v>
       </c>
+      <c r="B76" s="1"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>74</v>
       </c>
+      <c r="B77" s="1"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>75</v>
       </c>
+      <c r="B78" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>